<commit_message>
Workflow improvement (external context)
</commit_message>
<xml_diff>
--- a/demo/sample_emails.xlsx
+++ b/demo/sample_emails.xlsx
@@ -397,295 +397,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>output.subject</v>
+        <v>to</v>
       </c>
       <c r="B1" t="str">
-        <v>data</v>
+        <v>subject</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Missing Information Request - Jimmy Ellis</v>
-      </c>
-      <c r="B2" t="str" xml:space="preserve">
+        <v>jturner@example.com</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Request for Additional Information - Jimmy Ellis</v>
+      </c>
+      <c r="C2" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Jimmy,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our dataset and require some additional information from you.  Specifically, we are missing your job title. &lt;/p&gt;
-&lt;p&gt;Please provide this information at your earliest convenience. This will help us accurately represent your profile.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant at Blabla (Abu Dhabi - Training Focus)&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to complete our dataset for Blabla, a training company based in Abu Dhabi, UAE. We are currently reviewing your record and noticed some missing information.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your job title. Could you please provide this information at your earliest convenience? This will help us to better understand your profile and improve the accuracy of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
+        <v>brittanygarcia@example.com</v>
+      </c>
+      <c r="B3" t="str">
         <v>Data Completion Request - Blabla Training</v>
       </c>
-      <c r="B3" t="str" xml:space="preserve">
+      <c r="C3" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Hayden,&lt;/p&gt;
-&lt;p&gt;We are working to complete our dataset for Blabla Training and require some additional information from you. We are missing your mobile number. &lt;/p&gt;
-&lt;p&gt;Please provide your mobile number at your earliest convenience. This will help us ensure the accuracy and completeness of our records.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to enhance our dataset for Blabla Training. We are currently working to complete some missing information for our records.&lt;/p&gt;
+&lt;p&gt;We noticed that your record is missing a mobile number. Could you please provide this information at your earliest convenience? This will help us ensure the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Missing Information Request - Blabla Training</v>
-      </c>
-      <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Customer,&lt;/p&gt;
-&lt;p&gt;We are working to complete our records for Blabla Training and require a few more details to ensure accuracy.  Could you please provide the following information?&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;&lt;strong&gt;Name:&lt;/strong&gt; (Full Name)&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Nationality:&lt;/strong&gt;&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This will help us better understand our customer base and provide more relevant services.  Please reply to this email with the requested information at your earliest convenience.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa, Data Assistant&lt;/p&gt;</v>
+        <v>codylee@example.org</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Request for Missing Information - BlaBla Training</v>
+      </c>
+      <c r="C4" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Cody Lee,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm an assistant working to complete our dataset for BlaBla Training, a training company based in Abu Dhabi, UAE. We are currently working to enrich our records and would greatly appreciate it if you could provide a few missing details.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your name and nationality. This information is important for ensuring the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Could you please share this information at your earliest convenience?&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+BlaBla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>Missing Information Request - BlaBla Training Dataset</v>
-      </c>
-      <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Data Subject,&lt;/p&gt;
-&lt;p&gt;We are working to improve our training dataset for BlaBla, a training company based in Abu Dhabi. We have a record for you with the following information:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Email: chrisbailey@example.net&lt;/li&gt;
-&lt;li&gt;City: Port John&lt;/li&gt;
-&lt;li&gt;Nationality: Georgia&lt;/li&gt;
-&lt;li&gt;Passport: nd710587&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;To complete our record, could you please provide the following missing information:&lt;/p&gt;
+        <v>chrisbailey@example.net</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Data Completion Request - BlaBla Training</v>
+      </c>
+      <c r="C5" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Chris, &lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to enhance our training dataset for BlaBla Training, a company based in Abu Dhabi (UAE) specializing in training. &lt;/p&gt;
+&lt;p&gt;We are currently working to complete some missing information for our records.  Could you please provide the following details at your earliest convenience?&lt;/p&gt;
 &lt;ul&gt;
 &lt;li&gt;Name&lt;/li&gt;
 &lt;li&gt;Mobile Number&lt;/li&gt;
 &lt;/ul&gt;
-&lt;p&gt;Your cooperation is greatly appreciated. Please reply to this email with the requested details.&lt;/p&gt;
-&lt;p&gt;Thank you,&lt;/p&gt;
-&lt;p&gt;Luisa
-Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;This information is important for ensuring the accuracy and completeness of our data.  Thank you for your time and assistance.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, BlaBla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>Missing Information Request - William Duke</v>
-      </c>
-      <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear William Duke,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our dataset and require some additional information from you.  Specifically, we are missing your city of residence. &lt;/p&gt;
-&lt;p&gt;Please provide this information at your earliest convenience. &lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistance&lt;/p&gt;</v>
+        <v>thomascindy@example.net</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Request for Additional Information - William Duke</v>
+      </c>
+      <c r="C6" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Mr. Duke,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with data enrichment for Blabla, a training company based in Abu Dhabi, UAE. We are currently working to complete our records and would appreciate it if you could provide a few missing details.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your city of residence.  This information would help us better understand our client base.&lt;/p&gt;
+&lt;p&gt;Could you please share this information at your earliest convenience?&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Enrichment Assistant, Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
       <c r="A7" t="str">
-        <v>Missing Information Request - Blabla Training</v>
-      </c>
-      <c r="B7" t="str" xml:space="preserve">
+        <v>jpope@example.net</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Request for Missing Information - BlaBla Training</v>
+      </c>
+      <c r="C7" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Jordan,&lt;/p&gt;
-&lt;p&gt;We are working to complete our dataset for Blabla Training and require some additional information from you.  We are missing the following fields:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Job Title&lt;/li&gt;
-&lt;li&gt;Passport Number&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;Please provide these details at your earliest convenience.  Your cooperation is greatly appreciated.&lt;/p&gt;
-&lt;p&gt;Thank you,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant at BlaBla Training, a training company based in Abu Dhabi, UAE. We are currently working to complete our dataset and require a few additional details from you.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing information regarding your job title and passport details. Could you please provide this information at your earliest convenience?&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant
+BlaBla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="8" xml:space="preserve">
       <c r="A8" t="str">
-        <v>Missing Information Request - BlaBla Training Dataset</v>
-      </c>
-      <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Mr./Ms. Smithheidi,&lt;/p&gt;
-&lt;p&gt;We are working to complete our dataset on BlaBla Training and require some additional information to ensure accuracy.  We are missing your name and city. &lt;/p&gt;
-&lt;p&gt;Please provide this information at your earliest convenience. This will help us better understand and represent our diverse user base.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+        <v>smithheidi@example.net</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Request for Missing Information - BlaBla Training Dataset</v>
+      </c>
+      <c r="C8" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Mr./Ms. Heidi,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to enhance our BlaBla training dataset. We are currently working to complete the profiles of individuals associated with our training programs.&lt;/p&gt;
+&lt;p&gt;We noticed some missing information in your record and would greatly appreciate it if you could provide the following details:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;&lt;strong&gt;Name:&lt;/strong&gt; Full name for identification purposes.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;City:&lt;/strong&gt; Current city of residence.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;This information will help us improve the accuracy and completeness of our data. Please feel free to reply to this email with the requested details at your convenience.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, BlaBla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
       <c r="A9" t="str">
-        <v>Data Completion Request - Blabla Training</v>
-      </c>
-      <c r="B9" t="str" xml:space="preserve">
+        <v>rebeccanovak@example.com</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Data Completion Request - Missing Information for Laura Avila</v>
+      </c>
+      <c r="C9" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Laura Avila,&lt;/p&gt;
-&lt;p&gt;We are working to complete our dataset for Blabla Training, a training company based in Abu Dhabi. We noticed some missing information in your record and would appreciate it if you could provide the following:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Mobile Number&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This information is important for ensuring the accuracy and completeness of our data. Please reply to this email with the missing details at your earliest convenience.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa, Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with data enrichment for Blabla, a training company based in Abu Dhabi, UAE. We are currently working to complete our dataset and would greatly appreciate it if you could provide a few missing details.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your mobile number. This information is important for ensuring accurate and complete records.&lt;/p&gt;
+&lt;p&gt;Could you please share your mobile number at your earliest convenience?  Please feel free to reply to this email or let me know if you prefer an alternative method of providing this information.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant for Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="10" xml:space="preserve">
       <c r="A10" t="str">
-        <v>Missing Information Request - Patricia Kim</v>
-      </c>
-      <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Patricia,&lt;/p&gt;
-&lt;p&gt;We are working to complete our records for individuals associated with Blabla. We noticed some missing information in your record and would appreciate it if you could provide the following:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;City&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;Please reply to this email with the missing information. Thank you for your assistance!&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+        <v>michele29@example.net</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Data Completion Request - Missing City Information</v>
+      </c>
+      <c r="C10" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Patricia Kim,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with a data enrichment project for Blabla, a training company based in Abu Dhabi, UAE. We are working to complete our dataset and noticed some missing information in your record.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your city of residence. Could you please provide this information at your earliest convenience? This will help us ensure the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Enrichment Assistant&lt;/p&gt;</v>
       </c>
     </row>
     <row r="11" xml:space="preserve">
       <c r="A11" t="str">
-        <v>Missing Information Request - Blabla Training</v>
-      </c>
-      <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear cmartinez,&lt;/p&gt;
-&lt;p&gt;We are working to complete our dataset on Blabla Training, a company based in Abu Dhabi. We noticed some missing information in your record and would appreciate it if you could provide the following details:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Name&lt;/li&gt;
-&lt;li&gt;Nationality&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This information will help us build a more comprehensive profile of Blabla Training. Please let us know if you require any assistance.&lt;/p&gt;
-&lt;p&gt;Thank you for your time and cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+        <v>cmartinez@example.org</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Request for Missing Information - Blabla Training</v>
+      </c>
+      <c r="C11" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Mr. Martinez,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant with Blabla Training, based in Abu Dhabi, UAE. We are currently working to complete our dataset and require a few additional details from you.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your name and nationality. Could you please provide this information at your earliest convenience?&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Blabla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="12" xml:space="preserve">
       <c r="A12" t="str">
-        <v>Data Completion Request - Blabla Training</v>
-      </c>
-      <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Regina Smith,&lt;/p&gt;
-&lt;p&gt;We are working to enhance our dataset for Blabla Training and require some additional information to complete your record. Could you please provide the following details?&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;&lt;strong&gt;Job Title:&lt;/strong&gt; Your current job title.&lt;/li&gt;
-&lt;li&gt;&lt;strong&gt;Nationality:&lt;/strong&gt; Your nationality.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This information is important for us to accurately represent our diverse training participants. Please reply to this email with the requested details at your earliest convenience.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa, Data Assistant
-Blabla Training&lt;/p&gt;</v>
+        <v>amanda71@example.com</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Request for Missing Information - Regina Smith</v>
+      </c>
+      <c r="C12" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Regina,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with a data enrichment project for Blabla, a training company based in Abu Dhabi, UAE. We are working to complete our dataset and would greatly appreciate it if you could provide a few missing details from your record.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing information regarding your job title and nationality.  This information is important for us to accurately represent our diverse participant pool.&lt;/p&gt;
+&lt;p&gt;Could you please share this information at your earliest convenience?  Please feel free to reply to this email with the details.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance.  We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Enrichment Assistant&lt;/p&gt;</v>
       </c>
     </row>
     <row r="13" xml:space="preserve">
       <c r="A13" t="str">
-        <v>Missing Information Request - Candace Rodriguez</v>
-      </c>
-      <c r="B13" t="str" xml:space="preserve">
+        <v>taraflores@example.com</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Request for Missing Information - Candace Rodriguez</v>
+      </c>
+      <c r="C13" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Candace,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our dataset and require some additional information from you.  Specifically, we are missing your city of residence. &lt;/p&gt;
-&lt;p&gt;Could you please provide this information at your earliest convenience?  This will help us ensure the accuracy and completeness of our records.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistance&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to complete our dataset for Blabla, a training company based in Abu Dhabi, UAE. We are currently reviewing your record and noticed a few missing fields. Specifically, we are missing your city of residence.&lt;/p&gt;
+&lt;p&gt;Could you please provide this information at your earliest convenience? This will help us ensure the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="14" xml:space="preserve">
       <c r="A14" t="str">
-        <v>Request for Missing Information - John Dixon</v>
-      </c>
-      <c r="B14" t="str" xml:space="preserve">
+        <v>lori42@example.com</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Request for Additional Information - John Dixon</v>
+      </c>
+      <c r="C14" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear John Dixon,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our data records and noticed some missing information for your entry. Specifically, we are missing your nationality. &lt;/p&gt;
-&lt;p&gt;Could you please provide this information at your earliest convenience? This will help us ensure the accuracy and completeness of our database.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to complete our dataset for Blabla, a training company based in Abu Dhabi, UAE. We are currently reviewing your record and noticed some missing information.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your nationality. Could you please provide this information at your earliest convenience? This will help us ensure the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
       <c r="A15" t="str">
-        <v>Request for Missing Information - Valerie Jenkins</v>
-      </c>
-      <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Valerie,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our dataset and require some additional information from you.  Specifically, we are missing your job title. &lt;/p&gt;
-&lt;p&gt;Please provide this information at your earliest convenience.  This will help us accurately represent your profile.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+        <v>morenokaren@example.net</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Request for Additional Information - Valerie Jenkins</v>
+      </c>
+      <c r="C15" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Ms. Jenkins,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm a data assistant working to complete our dataset for Blabla, a training company based in Abu Dhabi, UAE. We are currently reviewing your record and noticed a few missing fields. Specifically, we are missing information regarding your job title.&lt;/p&gt;
+&lt;p&gt;Could you please provide details about your current role? This information is important for us to accurately represent our diverse participant pool.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla&lt;/p&gt;</v>
       </c>
     </row>
     <row r="16" xml:space="preserve">
       <c r="A16" t="str">
-        <v>Request for Missing Information - Diane Berger</v>
-      </c>
-      <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Diane,&lt;/p&gt;
-&lt;p&gt;We are currently working to complete our dataset and require a few more details for your record. Could you please provide your nationality and mobile number?&lt;/p&gt;
-&lt;p&gt;Thank you for your assistance.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant at Blabla (Abu Dhabi)&lt;/p&gt;</v>
+        <v>kristencastro@example.com</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Data Completion Request - BlaBla Training</v>
+      </c>
+      <c r="C16" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Diane Berger,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with data enrichment for BlaBla Training, a training company based in Abu Dhabi, UAE. We are working to complete our records and would greatly appreciate it if you could provide a few missing details from your profile.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your nationality and mobile number.  This information will help us ensure the accuracy and completeness of our database.&lt;/p&gt;
+&lt;p&gt;Could you please share this information at your earliest convenience?&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Enrichment Assistant, BlaBla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="17" xml:space="preserve">
       <c r="A17" t="str">
-        <v>Data Completion Request - Blabla Training</v>
-      </c>
-      <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;p&gt;Dear Joseph,&lt;/p&gt;
-&lt;p&gt;We are working to enhance our dataset for Blabla Training and require some additional information to complete your record. Could you please provide the following details?&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;City of residence&lt;/li&gt;
-&lt;li&gt;Nationality&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This information is important for our data analysis and reporting. Please reply to this email with the requested details at your earliest convenience.&lt;/p&gt;
-&lt;p&gt;Thank you for your cooperation.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+        <v>thomasbryan@example.net</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Data Completion Request - Blabla Training Dataset</v>
+      </c>
+      <c r="C17" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;p&gt;Dear Joseph Johnson,&lt;/p&gt;
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting with a project to enhance our training dataset for Blabla. We are currently working to complete some missing information for our records.&lt;/p&gt;
+&lt;p&gt;Your record indicates that the 'city' and 'nationality' fields are currently undefined. Could you please provide this information at your earliest convenience? This will greatly help us improve the accuracy and completeness of our data.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your cooperation.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Data Assistant, Blabla Training&lt;/p&gt;</v>
       </c>
     </row>
     <row r="18" xml:space="preserve">
       <c r="A18" t="str">
-        <v>Request for Missing Information - BlaBla Training Dataset</v>
-      </c>
-      <c r="B18" t="str" xml:space="preserve">
+        <v>paultrevino@example.org</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Data Completion Request - Blabla Training</v>
+      </c>
+      <c r="C18" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;p&gt;Dear Ann Smith,&lt;/p&gt;
-&lt;p&gt;We are working on expanding our training dataset for BlaBla, a training company based in Abu Dhabi. We noticed some missing information in your record and would appreciate it if you could provide the following details:&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Nationality&lt;/li&gt;
-&lt;li&gt;Mobile Number&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;This information is important for ensuring the accuracy and completeness of our data. Please let us know if you can provide this information at your earliest convenience.&lt;/p&gt;
-&lt;p&gt;Thank you for your time and assistance.&lt;/p&gt;
-&lt;p&gt;Sincerely,
-Luisa
-Data Assistant&lt;/p&gt;</v>
+&lt;p&gt;I hope this email finds you well.&lt;/p&gt;
+&lt;p&gt;My name is Luisa, and I'm assisting Blabla Training with enriching our dataset. We are currently working to improve our records and would greatly appreciate it if you could provide a few additional details.&lt;/p&gt;
+&lt;p&gt;Specifically, we are missing your nationality and mobile number.  This information will help us better understand our participant demographics.&lt;/p&gt;
+&lt;p&gt;If you are comfortable sharing this information, please let me know and I can provide a secure method for you to submit it.&lt;/p&gt;
+&lt;p&gt;Thank you for your time and assistance. We appreciate your contribution to Blabla Training.&lt;/p&gt;
+&lt;p&gt;Sincerely,
+Luisa
+Blabla Training (Abu Dhabi, UAE)&lt;/p&gt;</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>